<commit_message>
Refactor: Move Team from Assignments to Employees, fix Gantt chart display - Moved Team column from Assignments sheet to Employees sheet in Excel structure - Renamed Portfolio to Team throughout the application (dropdown, filtering, state) - Fixed Gantt chart CSS and rendering for proper visual timeline display - Added comprehensive Gantt chart styles with gradient bars and hover effects - Fixed file upload handling from landing page with proper module loading - Added direct upload button in main app header for easier file access - Improved date calculations for Gantt chart positioning - Enhanced error handling and user feedback
</commit_message>
<xml_diff>
--- a/ScheduleSample.xlsx
+++ b/ScheduleSample.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="114">
   <si>
     <t>Employee</t>
   </si>
@@ -21,274 +21,271 @@
     <t>Role</t>
   </si>
   <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Sarah Johnson</t>
+  </si>
+  <si>
+    <t>Senior Analyst</t>
+  </si>
+  <si>
+    <t>Financial System Migration</t>
+  </si>
+  <si>
+    <t>Compliance Review 2025</t>
+  </si>
+  <si>
+    <t>Michael Chen</t>
+  </si>
+  <si>
+    <t>Project Manager</t>
+  </si>
+  <si>
+    <t>Security Audit Q3</t>
+  </si>
+  <si>
+    <t>Emily Davis</t>
+  </si>
+  <si>
+    <t>Lead Auditor</t>
+  </si>
+  <si>
+    <t>James Wilson</t>
+  </si>
+  <si>
+    <t>Security Specialist</t>
+  </si>
+  <si>
+    <t>Network Security Implementation</t>
+  </si>
+  <si>
+    <t>Maria Garcia</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Cloud Infrastructure Upgrade</t>
+  </si>
+  <si>
+    <t>Data Analytics Platform</t>
+  </si>
+  <si>
+    <t>Robert Smith</t>
+  </si>
+  <si>
+    <t>Risk Manager</t>
+  </si>
+  <si>
+    <t>Lisa Anderson</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Customer Portal Enhancement</t>
+  </si>
+  <si>
+    <t>Process Automation Initiative</t>
+  </si>
+  <si>
+    <t>David Brown</t>
+  </si>
+  <si>
+    <t>Security Lead</t>
+  </si>
+  <si>
+    <t>Jennifer Taylor</t>
+  </si>
+  <si>
+    <t>Senior PM</t>
+  </si>
+  <si>
+    <t>Database Modernization</t>
+  </si>
+  <si>
+    <t>Thomas Martinez</t>
+  </si>
+  <si>
+    <t>Risk Analyst</t>
+  </si>
+  <si>
+    <t>Risk Assessment Framework</t>
+  </si>
+  <si>
+    <t>Amanda White</t>
+  </si>
+  <si>
+    <t>Business Analyst</t>
+  </si>
+  <si>
+    <t>Christopher Lee</t>
+  </si>
+  <si>
+    <t>Tech Lead</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
     <t>Team</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
-    <t>Sarah Johnson</t>
-  </si>
-  <si>
-    <t>Senior Analyst</t>
+    <t>Max Hours</t>
+  </si>
+  <si>
+    <t>Communication</t>
+  </si>
+  <si>
+    <t>Cybersecurity</t>
+  </si>
+  <si>
+    <t>Data Analysis</t>
+  </si>
+  <si>
+    <t>Financial Auditing</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Risk Assessment</t>
+  </si>
+  <si>
+    <t>EMP001</t>
+  </si>
+  <si>
+    <t>sarah.johnson@company.com</t>
+  </si>
+  <si>
+    <t>Operations</t>
+  </si>
+  <si>
+    <t>Advanced</t>
+  </si>
+  <si>
+    <t>Intermediate</t>
+  </si>
+  <si>
+    <t>Expert</t>
+  </si>
+  <si>
+    <t>Beginner</t>
+  </si>
+  <si>
+    <t>EMP002</t>
+  </si>
+  <si>
+    <t>michael.chen@company.com</t>
   </si>
   <si>
     <t>Finance</t>
   </si>
   <si>
-    <t>Financial System Migration</t>
-  </si>
-  <si>
-    <t>Compliance Review 2025</t>
-  </si>
-  <si>
-    <t>Michael Chen</t>
-  </si>
-  <si>
-    <t>Project Manager</t>
+    <t>None</t>
+  </si>
+  <si>
+    <t>EMP003</t>
+  </si>
+  <si>
+    <t>emily.davis@company.com</t>
+  </si>
+  <si>
+    <t>EMP004</t>
+  </si>
+  <si>
+    <t>james.wilson@company.com</t>
   </si>
   <si>
     <t>IT</t>
   </si>
   <si>
-    <t>Security Audit Q3</t>
-  </si>
-  <si>
-    <t>Emily Davis</t>
-  </si>
-  <si>
-    <t>Lead Auditor</t>
-  </si>
-  <si>
-    <t>James Wilson</t>
-  </si>
-  <si>
-    <t>Security Specialist</t>
+    <t>EMP005</t>
+  </si>
+  <si>
+    <t>maria.garcia@company.com</t>
+  </si>
+  <si>
+    <t>EMP006</t>
+  </si>
+  <si>
+    <t>robert.smith@company.com</t>
+  </si>
+  <si>
+    <t>EMP007</t>
+  </si>
+  <si>
+    <t>lisa.anderson@company.com</t>
+  </si>
+  <si>
+    <t>EMP008</t>
+  </si>
+  <si>
+    <t>david.brown@company.com</t>
+  </si>
+  <si>
+    <t>Analytics</t>
+  </si>
+  <si>
+    <t>EMP009</t>
+  </si>
+  <si>
+    <t>jennifer.taylor@company.com</t>
+  </si>
+  <si>
+    <t>EMP010</t>
+  </si>
+  <si>
+    <t>thomas.martinez@company.com</t>
+  </si>
+  <si>
+    <t>PMO</t>
+  </si>
+  <si>
+    <t>EMP011</t>
+  </si>
+  <si>
+    <t>amanda.white@company.com</t>
+  </si>
+  <si>
+    <t>EMP012</t>
+  </si>
+  <si>
+    <t>christopher.lee@company.com</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Portfolio</t>
+  </si>
+  <si>
+    <t>Required Skills</t>
+  </si>
+  <si>
+    <t>PROJ000</t>
+  </si>
+  <si>
+    <t>Time Off</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>PROJ001</t>
   </si>
   <si>
     <t>IT Security</t>
-  </si>
-  <si>
-    <t>Network Security Implementation</t>
-  </si>
-  <si>
-    <t>Maria Garcia</t>
-  </si>
-  <si>
-    <t>Data Analyst</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>Cloud Infrastructure Upgrade</t>
-  </si>
-  <si>
-    <t>Data Analytics Platform</t>
-  </si>
-  <si>
-    <t>Robert Smith</t>
-  </si>
-  <si>
-    <t>Risk Manager</t>
-  </si>
-  <si>
-    <t>Risk</t>
-  </si>
-  <si>
-    <t>Lisa Anderson</t>
-  </si>
-  <si>
-    <t>PM</t>
-  </si>
-  <si>
-    <t>Operations</t>
-  </si>
-  <si>
-    <t>Customer Portal Enhancement</t>
-  </si>
-  <si>
-    <t>Process Automation Initiative</t>
-  </si>
-  <si>
-    <t>David Brown</t>
-  </si>
-  <si>
-    <t>Security Lead</t>
-  </si>
-  <si>
-    <t>Jennifer Taylor</t>
-  </si>
-  <si>
-    <t>Senior PM</t>
-  </si>
-  <si>
-    <t>PMO</t>
-  </si>
-  <si>
-    <t>Database Modernization</t>
-  </si>
-  <si>
-    <t>Thomas Martinez</t>
-  </si>
-  <si>
-    <t>Risk Analyst</t>
-  </si>
-  <si>
-    <t>Risk Assessment Framework</t>
-  </si>
-  <si>
-    <t>Amanda White</t>
-  </si>
-  <si>
-    <t>Business Analyst</t>
-  </si>
-  <si>
-    <t>Christopher Lee</t>
-  </si>
-  <si>
-    <t>Tech Lead</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Max Hours</t>
-  </si>
-  <si>
-    <t>Communication</t>
-  </si>
-  <si>
-    <t>Cybersecurity</t>
-  </si>
-  <si>
-    <t>Data Analysis</t>
-  </si>
-  <si>
-    <t>Financial Auditing</t>
-  </si>
-  <si>
-    <t>Project Management</t>
-  </si>
-  <si>
-    <t>Risk Assessment</t>
-  </si>
-  <si>
-    <t>EMP001</t>
-  </si>
-  <si>
-    <t>sarah.johnson@company.com</t>
-  </si>
-  <si>
-    <t>Advanced</t>
-  </si>
-  <si>
-    <t>Intermediate</t>
-  </si>
-  <si>
-    <t>Expert</t>
-  </si>
-  <si>
-    <t>Beginner</t>
-  </si>
-  <si>
-    <t>EMP002</t>
-  </si>
-  <si>
-    <t>michael.chen@company.com</t>
-  </si>
-  <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>EMP003</t>
-  </si>
-  <si>
-    <t>emily.davis@company.com</t>
-  </si>
-  <si>
-    <t>EMP004</t>
-  </si>
-  <si>
-    <t>james.wilson@company.com</t>
-  </si>
-  <si>
-    <t>EMP005</t>
-  </si>
-  <si>
-    <t>maria.garcia@company.com</t>
-  </si>
-  <si>
-    <t>EMP006</t>
-  </si>
-  <si>
-    <t>robert.smith@company.com</t>
-  </si>
-  <si>
-    <t>EMP007</t>
-  </si>
-  <si>
-    <t>lisa.anderson@company.com</t>
-  </si>
-  <si>
-    <t>EMP008</t>
-  </si>
-  <si>
-    <t>david.brown@company.com</t>
-  </si>
-  <si>
-    <t>EMP009</t>
-  </si>
-  <si>
-    <t>jennifer.taylor@company.com</t>
-  </si>
-  <si>
-    <t>EMP010</t>
-  </si>
-  <si>
-    <t>thomas.martinez@company.com</t>
-  </si>
-  <si>
-    <t>EMP011</t>
-  </si>
-  <si>
-    <t>amanda.white@company.com</t>
-  </si>
-  <si>
-    <t>EMP012</t>
-  </si>
-  <si>
-    <t>christopher.lee@company.com</t>
-  </si>
-  <si>
-    <t>Start Date</t>
-  </si>
-  <si>
-    <t>End Date</t>
-  </si>
-  <si>
-    <t>Portfolio</t>
-  </si>
-  <si>
-    <t>Required Skills</t>
-  </si>
-  <si>
-    <t>PROJ000</t>
-  </si>
-  <si>
-    <t>Time Off</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>PROJ001</t>
   </si>
   <si>
     <t>Cybersecurity, Risk Assessment, Data Analysis</t>
@@ -642,58 +639,55 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
+      <c r="D1" s="2">
+        <v>46027.0</v>
       </c>
       <c r="E1" s="2">
-        <v>46027.0</v>
+        <v>46034.0</v>
       </c>
       <c r="F1" s="2">
-        <v>46034.0</v>
+        <v>46041.0</v>
       </c>
       <c r="G1" s="2">
-        <v>46041.0</v>
+        <v>46048.0</v>
       </c>
       <c r="H1" s="2">
-        <v>46048.0</v>
+        <v>46055.0</v>
       </c>
       <c r="I1" s="2">
-        <v>46055.0</v>
+        <v>46062.0</v>
       </c>
       <c r="J1" s="2">
-        <v>46062.0</v>
+        <v>46069.0</v>
       </c>
       <c r="K1" s="2">
-        <v>46069.0</v>
+        <v>46076.0</v>
       </c>
       <c r="L1" s="2">
-        <v>46076.0</v>
+        <v>46083.0</v>
       </c>
       <c r="M1" s="2">
-        <v>46083.0</v>
+        <v>46090.0</v>
       </c>
       <c r="N1" s="2">
-        <v>46090.0</v>
+        <v>46097.0</v>
       </c>
       <c r="O1" s="2">
-        <v>46097.0</v>
-      </c>
-      <c r="P1" s="2">
         <v>46104.0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+      <c r="D2" s="1">
+        <v>20.0</v>
       </c>
       <c r="E2" s="1">
         <v>20.0</v>
@@ -726,24 +720,21 @@
         <v>20.0</v>
       </c>
       <c r="O2" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="P2" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
+      <c r="D3" s="1">
+        <v>10.0</v>
       </c>
       <c r="E3" s="1">
         <v>10.0</v>
@@ -767,7 +758,7 @@
         <v>10.0</v>
       </c>
       <c r="L3" s="1">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="M3" s="1">
         <v>0.0</v>
@@ -778,22 +769,19 @@
       <c r="O3" s="1">
         <v>0.0</v>
       </c>
-      <c r="P3" s="1">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
+      <c r="D4" s="1">
+        <v>25.0</v>
       </c>
       <c r="E4" s="1">
         <v>25.0</v>
@@ -826,24 +814,21 @@
         <v>25.0</v>
       </c>
       <c r="O4" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="P4" s="1">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <v>30.0</v>
       </c>
       <c r="E5" s="1">
         <v>30.0</v>
@@ -878,22 +863,19 @@
       <c r="O5" s="1">
         <v>30.0</v>
       </c>
-      <c r="P5" s="1">
-        <v>30.0</v>
-      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
+      </c>
+      <c r="D6" s="1">
+        <v>15.0</v>
       </c>
       <c r="E6" s="1">
         <v>15.0</v>
@@ -926,24 +908,21 @@
         <v>15.0</v>
       </c>
       <c r="O6" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="P6" s="1">
         <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20.0</v>
       </c>
       <c r="E7" s="1">
         <v>20.0</v>
@@ -976,24 +955,21 @@
         <v>20.0</v>
       </c>
       <c r="O7" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="P7" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="1">
+        <v>20.0</v>
       </c>
       <c r="E8" s="1">
         <v>20.0</v>
@@ -1026,24 +1002,21 @@
         <v>20.0</v>
       </c>
       <c r="O8" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="P8" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15.0</v>
       </c>
       <c r="E9" s="1">
         <v>15.0</v>
@@ -1076,24 +1049,21 @@
         <v>15.0</v>
       </c>
       <c r="O9" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="P9" s="1">
         <v>15.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
+      </c>
+      <c r="D10" s="1">
+        <v>25.0</v>
       </c>
       <c r="E10" s="1">
         <v>25.0</v>
@@ -1126,24 +1096,21 @@
         <v>25.0</v>
       </c>
       <c r="O10" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="P10" s="1">
         <v>25.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
+        <v>20.0</v>
       </c>
       <c r="E11" s="1">
         <v>20.0</v>
@@ -1170,7 +1137,7 @@
         <v>20.0</v>
       </c>
       <c r="M11" s="1">
-        <v>20.0</v>
+        <v>0.0</v>
       </c>
       <c r="N11" s="1">
         <v>0.0</v>
@@ -1178,22 +1145,19 @@
       <c r="O11" s="1">
         <v>0.0</v>
       </c>
-      <c r="P11" s="1">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>15.0</v>
       </c>
       <c r="E12" s="1">
         <v>15.0</v>
@@ -1226,24 +1190,21 @@
         <v>15.0</v>
       </c>
       <c r="O12" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="P12" s="1">
         <v>15.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
+      </c>
+      <c r="D13" s="1">
+        <v>30.0</v>
       </c>
       <c r="E13" s="1">
         <v>30.0</v>
@@ -1278,22 +1239,19 @@
       <c r="O13" s="1">
         <v>30.0</v>
       </c>
-      <c r="P13" s="1">
-        <v>30.0</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
+      </c>
+      <c r="D14" s="1">
+        <v>15.0</v>
       </c>
       <c r="E14" s="1">
         <v>15.0</v>
@@ -1326,24 +1284,21 @@
         <v>15.0</v>
       </c>
       <c r="O14" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="P14" s="1">
         <v>15.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="D15" s="1">
+        <v>20.0</v>
       </c>
       <c r="E15" s="1">
         <v>20.0</v>
@@ -1376,24 +1331,21 @@
         <v>20.0</v>
       </c>
       <c r="O15" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="P15" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="D16" s="1">
+        <v>25.0</v>
       </c>
       <c r="E16" s="1">
         <v>25.0</v>
@@ -1426,24 +1378,21 @@
         <v>25.0</v>
       </c>
       <c r="O16" s="1">
-        <v>25.0</v>
-      </c>
-      <c r="P16" s="1">
         <v>25.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="D17" s="1">
+        <v>20.0</v>
       </c>
       <c r="E17" s="1">
         <v>20.0</v>
@@ -1476,24 +1425,21 @@
         <v>20.0</v>
       </c>
       <c r="O17" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="P17" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
+      </c>
+      <c r="D18" s="1">
+        <v>10.0</v>
       </c>
       <c r="E18" s="1">
         <v>10.0</v>
@@ -1520,7 +1466,7 @@
         <v>10.0</v>
       </c>
       <c r="M18" s="1">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="N18" s="1">
         <v>0.0</v>
@@ -1528,22 +1474,19 @@
       <c r="O18" s="1">
         <v>0.0</v>
       </c>
-      <c r="P18" s="1">
-        <v>0.0</v>
-      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
+      </c>
+      <c r="D19" s="1">
+        <v>20.0</v>
       </c>
       <c r="E19" s="1">
         <v>20.0</v>
@@ -1576,24 +1519,21 @@
         <v>20.0</v>
       </c>
       <c r="O19" s="1">
-        <v>20.0</v>
-      </c>
-      <c r="P19" s="1">
         <v>20.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="D20" s="1">
+        <v>15.0</v>
       </c>
       <c r="E20" s="1">
         <v>15.0</v>
@@ -1626,9 +1566,6 @@
         <v>15.0</v>
       </c>
       <c r="O20" s="1">
-        <v>15.0</v>
-      </c>
-      <c r="P20" s="1">
         <v>15.0</v>
       </c>
     </row>
@@ -1649,418 +1586,457 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="1">
+        <v>49</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="1">
         <v>40.0</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F2" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="1">
+        <v>56</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="1">
         <v>40.0</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="J3" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D4" s="1">
+        <v>60</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E4" s="1">
         <v>35.0</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="1">
+        <v>62</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="1">
         <v>40.0</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" s="1">
+        <v>65</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="1">
         <v>40.0</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="D7" s="1">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1">
         <v>40.0</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>58</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="1">
+        <v>69</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="1">
         <v>35.0</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F8" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="1">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="1">
         <v>40.0</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F9" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>58</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="1">
+        <v>74</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="1">
         <v>40.0</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D11" s="1">
+        <v>76</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E11" s="1">
         <v>40.0</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>58</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="1">
+        <v>79</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="1">
         <v>35.0</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>58</v>
+        <v>53</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D13" s="1">
+        <v>81</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1">
         <v>40.0</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>60</v>
-      </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -2080,30 +2056,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3">
         <v>45658.0</v>
@@ -2112,18 +2088,18 @@
         <v>46022.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="3">
         <v>45901.0</v>
@@ -2132,18 +2108,18 @@
         <v>45991.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3">
         <v>45884.0</v>
@@ -2152,18 +2128,18 @@
         <v>46006.0</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3">
         <v>45901.0</v>
@@ -2172,18 +2148,18 @@
         <v>46053.0</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" s="3">
         <v>45870.0</v>
@@ -2192,18 +2168,18 @@
         <v>45961.0</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C7" s="3">
         <v>45915.0</v>
@@ -2212,18 +2188,18 @@
         <v>46081.0</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C8" s="3">
         <v>45931.0</v>
@@ -2232,18 +2208,18 @@
         <v>46112.0</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3">
         <v>45870.0</v>
@@ -2252,18 +2228,18 @@
         <v>45976.0</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C10" s="3">
         <v>45901.0</v>
@@ -2272,18 +2248,18 @@
         <v>46022.0</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C11" s="3">
         <v>45884.0</v>
@@ -2292,18 +2268,18 @@
         <v>46037.0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C12" s="3">
         <v>45931.0</v>
@@ -2312,10 +2288,10 @@
         <v>46068.0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>